<commit_message>
Goorin tech and loader
</commit_message>
<xml_diff>
--- a/Excel/Goorin Brothers/04.03.2022 Goorin Brothers — техничка.xlsx
+++ b/Excel/Goorin Brothers/04.03.2022 Goorin Brothers — техничка.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Goorin Brothers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22A0C246-06EF-45E3-9B3B-C05E9F2623F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F5B1487-1F1B-447D-AFFB-8DA779732C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3EC64EE7-0AA4-4975-80A2-6A9A2179DFEE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B64D72C5-9703-48B7-97DE-CE85725AC981}"/>
   </bookViews>
   <sheets>
     <sheet name="Техничка Goorin Brothers" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2573" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2573" uniqueCount="442">
   <si>
     <t>Артикул на этикетке</t>
   </si>
@@ -906,7 +906,7 @@
     <t>201-3001</t>
   </si>
   <si>
-    <t>синий / белый</t>
+    <t>100% полиэстер</t>
   </si>
   <si>
     <t>91-133-34</t>
@@ -915,9 +915,6 @@
     <t>201-3002</t>
   </si>
   <si>
-    <t>белый / розовый</t>
-  </si>
-  <si>
     <t>91-693-09</t>
   </si>
   <si>
@@ -955,9 +952,6 @@
   </si>
   <si>
     <t>песочный</t>
-  </si>
-  <si>
-    <t>100% полиэстер</t>
   </si>
   <si>
     <t>91-698-02</t>
@@ -1649,7 +1643,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E1C3519-DE73-47AB-B6DF-BC8C70E4269B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD11F925-6C40-4F90-875A-9CB63B65D211}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1699,7 +1693,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F4040BD-83DC-427E-AC77-88EEEAC8E25E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E40F9CB9-D53D-4703-8AEB-EA7BA34AA26C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1749,7 +1743,7 @@
         <xdr:cNvPr id="4" name="Рисунок 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C44C7E55-C6A8-4351-96B9-AF35103279C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37E4F55D-BB4C-4049-8C18-E98F78297B9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1799,7 +1793,7 @@
         <xdr:cNvPr id="5" name="Рисунок 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFE02731-8506-413D-9C8B-5502FB16882D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8D6A4F8-77C2-4752-B286-C4E85E70421C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1849,7 +1843,7 @@
         <xdr:cNvPr id="6" name="Рисунок 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2407B0F1-DFFE-430E-898A-621F62219F04}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF9759A7-73F3-4AB8-BFF4-72BE400AF8A2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1899,7 +1893,7 @@
         <xdr:cNvPr id="7" name="Рисунок 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8E97C65-48F6-4382-9690-74127349D302}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{290490A4-9D10-4550-8617-F966E5E925AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1949,7 +1943,7 @@
         <xdr:cNvPr id="8" name="Рисунок 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78F20C41-69AF-4E43-A54F-1E4CF30A2D09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{490F6D8B-689C-4EE8-AC6F-2FE17F3EEA02}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1999,7 +1993,7 @@
         <xdr:cNvPr id="9" name="Рисунок 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5EC1B987-9127-4B64-BCF2-72DB92CA2A8C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF972351-0D1E-42D8-9976-224241FA805F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2049,7 +2043,7 @@
         <xdr:cNvPr id="10" name="Рисунок 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44629723-1E93-44B1-811F-CDCBEDF330EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57A8DDAA-79FA-4A80-8E04-527712851106}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2099,7 +2093,7 @@
         <xdr:cNvPr id="11" name="Рисунок 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBF36190-3DA5-4DD3-A759-5CC2E6B516EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{034B2219-E6F8-4B66-AC63-D4AEC289F50E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2149,7 +2143,7 @@
         <xdr:cNvPr id="12" name="Рисунок 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56B8F88F-AF36-4ECD-8909-2408BBB4BA4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1048E98D-786D-489B-B72D-72EBFAFA09CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2199,7 +2193,7 @@
         <xdr:cNvPr id="13" name="Рисунок 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F1B6010-CE9A-423D-B68A-27B4C50ECCC8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{078C6A09-DD7B-4959-9209-F6F3CFD9C585}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2249,7 +2243,7 @@
         <xdr:cNvPr id="14" name="Рисунок 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD539940-8D0F-48EE-9D5D-E2E5A31EFAD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0909DDD4-D715-49BA-83FC-177F0AF226F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2299,7 +2293,7 @@
         <xdr:cNvPr id="15" name="Рисунок 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6FC0F5-B08C-43F9-B77A-792EE4DEBBF1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9514DD54-5B5A-4029-9425-3B77AE8CE0A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2349,7 +2343,7 @@
         <xdr:cNvPr id="16" name="Рисунок 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F48C6FD3-299D-4985-906F-6ED9510F90C5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C665C5AF-D426-4100-BBC9-FC61F31A90A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2399,7 +2393,7 @@
         <xdr:cNvPr id="17" name="Рисунок 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCF1E1E0-79B2-4C2E-9594-DA7A97E0EE59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3A8B75D-738E-42DC-B40B-22B4F6C93B6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2449,7 +2443,7 @@
         <xdr:cNvPr id="18" name="Рисунок 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07D05EB1-7713-488E-8426-825C91A14EE9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C00CD18-DF32-4A12-A2EC-CF3A1764F447}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2499,7 +2493,7 @@
         <xdr:cNvPr id="19" name="Рисунок 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7A582C4-140F-42EE-AB4D-11BAB822B027}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8EABF78-6D00-4BBB-AF17-E0D3D81AB735}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2549,7 +2543,7 @@
         <xdr:cNvPr id="20" name="Рисунок 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6571E3CA-3428-4EFB-BDAA-B6866015C487}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F4218AB-2FC7-4E8F-802E-0A24588D79FF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2599,7 +2593,7 @@
         <xdr:cNvPr id="21" name="Рисунок 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE18EE2-23FB-4B88-A5E0-7EA0C7522F31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E754A1E8-CFE4-41EC-B29A-2534A71E8027}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2649,7 +2643,7 @@
         <xdr:cNvPr id="22" name="Рисунок 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B49D5113-5D18-4755-813B-9EA3C5098958}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5767324-B7E1-4D8B-A52A-00FD9856BA9C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2699,7 +2693,7 @@
         <xdr:cNvPr id="23" name="Рисунок 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB407153-0D58-4F2C-BDE7-3B3247743005}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57337EEE-D925-459F-92EC-1FA8B0098F18}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2749,7 +2743,7 @@
         <xdr:cNvPr id="24" name="Рисунок 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{856BB245-1300-4B71-8158-F16E03B1620D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{906302AE-A338-495F-9CCC-3B98C0305234}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2799,7 +2793,7 @@
         <xdr:cNvPr id="25" name="Рисунок 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFAE27EE-96C9-4AFB-A797-8A9CFD8CDCB6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{314AE43C-58E9-4A61-AC8F-D68E7B1CB3F2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2849,7 +2843,7 @@
         <xdr:cNvPr id="26" name="Рисунок 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14FADE2-B898-4081-B486-438AA5F69BF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{618B63C0-FA31-47C9-918E-A80031571AA2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2899,7 +2893,7 @@
         <xdr:cNvPr id="27" name="Рисунок 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF02A1D5-5E51-463D-AF07-7D29911FA744}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21285B1A-BA61-4FF9-A6F8-0E7125C82732}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2949,7 +2943,7 @@
         <xdr:cNvPr id="28" name="Рисунок 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1305496C-0DC5-49A8-ABD1-45A8FB6DF372}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F59C4CE-DEC8-43CB-AE8F-2366D8C66142}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2999,7 +2993,7 @@
         <xdr:cNvPr id="29" name="Рисунок 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9BC0E80-33F1-4BD1-80C8-35C699DD293B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE494CA7-092A-437F-982F-B4A85E2C2491}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3049,7 +3043,7 @@
         <xdr:cNvPr id="30" name="Рисунок 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75B97F51-3D41-4612-85ED-2D07982262C2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9AB4DD0-D9DE-4E94-A194-49295049AA3A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3099,7 +3093,7 @@
         <xdr:cNvPr id="31" name="Рисунок 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{592AA0DF-A000-4A21-B965-51A31E4539A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4D3185B-33EF-4202-8A4B-D512A07850A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3149,7 +3143,7 @@
         <xdr:cNvPr id="32" name="Рисунок 31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE3FF3EC-B71C-4A0A-B02B-21ED0BC6DE57}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E05DEA0-D286-4373-ADB0-F340D5CD250E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3199,7 +3193,7 @@
         <xdr:cNvPr id="33" name="Рисунок 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B98D583-D6A5-4C91-830F-50C5C8BAB3F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7B892EF-60D8-4E94-BE5C-F30DC63F530F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3249,7 +3243,7 @@
         <xdr:cNvPr id="34" name="Рисунок 33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1BA8174-1DBD-40AE-925C-45184FAFC108}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DFBF58E-2B01-46C1-8A9A-51BF1FB77756}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3299,7 +3293,7 @@
         <xdr:cNvPr id="35" name="Рисунок 34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C93AB346-7C05-4656-84CE-21A17A371ADD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89A17E03-1F38-49C4-A3BB-12E47D63D8BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3349,7 +3343,7 @@
         <xdr:cNvPr id="36" name="Рисунок 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C3F4B2F-41CA-456B-996E-F20A35DB7A7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA9F4061-6E36-4606-8D8D-9213BD02BC8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3399,7 +3393,7 @@
         <xdr:cNvPr id="37" name="Рисунок 36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17961731-0A10-4396-B67E-D05BADA9C184}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2EA8938-93D4-471C-AD29-322C60E6C584}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3449,7 +3443,7 @@
         <xdr:cNvPr id="38" name="Рисунок 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14249A46-A381-418A-8537-B7118890CC95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A340607B-7CEC-49C8-A20F-C983021A04A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3499,7 +3493,7 @@
         <xdr:cNvPr id="39" name="Рисунок 38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA7834D9-7357-4940-AF86-4AC2A1C49464}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAC0BF35-B165-4CEA-87AF-64B61D0AAD10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3549,7 +3543,7 @@
         <xdr:cNvPr id="40" name="Рисунок 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D0A47D4-9EBF-4A0E-92F6-1C9A1A4FD52E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E6A5FD8-A6A0-430C-967F-CD9695AC983F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3599,7 +3593,7 @@
         <xdr:cNvPr id="41" name="Рисунок 40">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{149A9882-B7E3-4B1E-8676-B96040F52E87}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E763FF2-3C81-4FDA-A483-9BBB0CD5A850}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3649,7 +3643,7 @@
         <xdr:cNvPr id="42" name="Рисунок 41">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78D3C6BD-D62A-4592-BC58-661D2C19E87A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41BCF892-6691-467D-9ABF-BEA916EF8158}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3699,7 +3693,7 @@
         <xdr:cNvPr id="43" name="Рисунок 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE1C7ED4-1EFF-428A-84AF-1CA1E508DE37}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF3032CB-16C9-4152-9201-B32E5BB31A55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3749,7 +3743,7 @@
         <xdr:cNvPr id="44" name="Рисунок 43">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE692E1-2635-4AAE-AD5B-259B6C099FD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{728F0E94-1B4B-4F37-B043-60BFFBA8CA77}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3799,7 +3793,7 @@
         <xdr:cNvPr id="45" name="Рисунок 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F700FBC-2C47-464D-9A07-7884DE0F3C9E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C28ED2-11D3-410F-A1B2-89228E5C3370}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3849,7 +3843,7 @@
         <xdr:cNvPr id="46" name="Рисунок 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC8E614-49D9-4535-9528-DBB6DCAF0691}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDDF47E5-7D5C-4FC6-BB6F-6301DE6B6B3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3899,7 +3893,7 @@
         <xdr:cNvPr id="47" name="Рисунок 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BA505F3-CD89-4F6A-AB23-F1F2EC36682B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17321456-D9D2-4283-8547-D26FBF466906}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3949,7 +3943,7 @@
         <xdr:cNvPr id="48" name="Рисунок 47">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4926B809-85D5-4718-B38C-C1D921145BDD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8859A034-E209-48A9-8045-2893BAF1D989}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3999,7 +3993,7 @@
         <xdr:cNvPr id="49" name="Рисунок 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34065A0E-AD81-4080-9018-ED7248CA7592}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328F6668-1A40-4A03-8310-5D2BA8CF481F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4049,7 +4043,7 @@
         <xdr:cNvPr id="50" name="Рисунок 49">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E812E1AE-61B1-4FB3-947A-943505BF96C3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DD96367-09F2-4C26-96DB-2C294C64CAFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4099,7 +4093,7 @@
         <xdr:cNvPr id="51" name="Рисунок 50">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A01D984-3993-4086-9CBE-C80DCCB74BBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E368396A-C13A-4932-8F92-0C532D9B139A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4149,7 +4143,7 @@
         <xdr:cNvPr id="52" name="Рисунок 51">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E4849AE-A14C-4CD0-9A37-3DC4D4D3B44D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{366B3403-EB11-489A-9A21-55A8A362925F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4199,7 +4193,7 @@
         <xdr:cNvPr id="53" name="Рисунок 52">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25A3D2A2-60F1-4269-8145-553DEF4AD630}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BB26C3B-F5DE-45D5-BEFE-3EC5AF5D441F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4249,7 +4243,7 @@
         <xdr:cNvPr id="54" name="Рисунок 53">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C18027AC-0F64-4304-8FD9-D2BAAC65F7FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCB70B83-8E37-476B-854F-3EA5B50C3AB7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4299,7 +4293,7 @@
         <xdr:cNvPr id="55" name="Рисунок 54">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{833625AD-4BE8-4E11-A956-E41750E344B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33B3E244-B968-47DF-9B91-DBE24920DB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4349,7 +4343,7 @@
         <xdr:cNvPr id="56" name="Рисунок 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEDE2D93-5051-4B8E-9F64-BC2A7AD68693}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49E53725-02D9-4346-B697-06A2B67A4949}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4399,7 +4393,7 @@
         <xdr:cNvPr id="57" name="Рисунок 56">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBB46BA1-A601-438A-96D2-D4A03311313A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{914E7C9F-23AA-488C-B45F-9F78CCD75837}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4449,7 +4443,7 @@
         <xdr:cNvPr id="58" name="Рисунок 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F352F206-20C4-4838-A15A-1AF729634078}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F476691C-CBB2-426D-8296-580F3777EDB8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4499,7 +4493,7 @@
         <xdr:cNvPr id="59" name="Рисунок 58">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F4C51AD-1F45-4D89-A8C1-763170977360}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E68868E-6E97-453D-BD2E-4A57EB84831E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4549,7 +4543,7 @@
         <xdr:cNvPr id="60" name="Рисунок 59">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{895A7E9E-23B0-45A8-B755-E3404AAB0440}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A733CE93-BA62-4E20-B9FA-F7EECA161969}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4599,7 +4593,7 @@
         <xdr:cNvPr id="61" name="Рисунок 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EF25528-DBB8-498B-921F-6F58E63BE835}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50A58B2C-FE06-4FD2-B0E3-15BF3828D512}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4649,7 +4643,7 @@
         <xdr:cNvPr id="62" name="Рисунок 61">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8E144A4-FC88-43E1-9E1D-AC9DBD4B65D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E4DBE32-0C71-402D-8A2D-C2C771CD636B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4699,7 +4693,7 @@
         <xdr:cNvPr id="63" name="Рисунок 62">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{776105E8-4217-45D9-8729-F4A1403CB2B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DF5EFF0-381C-4073-A0A7-B087B29CE4EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4749,7 +4743,7 @@
         <xdr:cNvPr id="64" name="Рисунок 63">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D04E053-65E2-4785-96A7-D92663C27EE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F8E07D-4E19-4F2E-86A0-6B8732BD0839}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4799,7 +4793,7 @@
         <xdr:cNvPr id="65" name="Рисунок 64">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D38AD081-18B7-4C82-9094-E778CB70DBBA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D370FC3-EA82-4A54-8E61-B6F893920CF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4849,7 +4843,7 @@
         <xdr:cNvPr id="66" name="Рисунок 65">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0693A1B9-6EAE-439C-9777-2E93937C2237}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4A0D162-EBF0-4D45-8522-7E7B82749940}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4899,7 +4893,7 @@
         <xdr:cNvPr id="67" name="Рисунок 66">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89CE49B3-5858-4E62-A49D-E63758A2AF56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C61E24F-9CE8-4D92-B678-68C57F21FA82}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4949,7 +4943,7 @@
         <xdr:cNvPr id="68" name="Рисунок 67">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{494E78DB-3393-4476-85DD-12F490868F6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4C24BD5-62DA-42EC-A165-64E578CF0E6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4999,7 +4993,7 @@
         <xdr:cNvPr id="69" name="Рисунок 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E28BE7E-2786-4322-986C-5A0435029E68}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9242C521-DDD7-4CEC-B2B5-566636C5E702}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5049,7 +5043,7 @@
         <xdr:cNvPr id="70" name="Рисунок 69">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44443266-681F-461F-8F70-FFF8665059B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A099039-4E4A-4C18-B614-48D11A67D072}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5099,7 +5093,7 @@
         <xdr:cNvPr id="71" name="Рисунок 70">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34389E5F-889A-4EF2-8BD3-5BAD5B373A40}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B688810A-4109-4917-B074-D149692C1452}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5149,7 +5143,7 @@
         <xdr:cNvPr id="72" name="Рисунок 71">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41DE4261-0ACA-4CCB-A85A-57B9943D7B36}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89C28777-81BD-4D51-B366-79BADA682FB6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5199,7 +5193,7 @@
         <xdr:cNvPr id="73" name="Рисунок 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F98967E-B1E6-4A09-B737-52A78EC6CFBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{081F4E10-E60B-48FE-BA20-4E374D540CA7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5249,7 +5243,7 @@
         <xdr:cNvPr id="74" name="Рисунок 73">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70608551-AB58-4A1D-82AC-ACD620DBF10F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C15E1DB-BBC9-452F-A77F-A2CC717B7332}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5299,7 +5293,7 @@
         <xdr:cNvPr id="75" name="Рисунок 74">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11C0B61A-829D-4D95-AC3D-5EDC4EED65B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE61BF8E-CBCE-481B-9213-B52AB162EF53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5349,7 +5343,7 @@
         <xdr:cNvPr id="76" name="Рисунок 75">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C3AD359-9AE4-447C-8CF4-02B0DA8718AB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{741B843F-A666-44B5-B9E3-62217828AB8C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5399,7 +5393,7 @@
         <xdr:cNvPr id="77" name="Рисунок 76">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5FD119E-60D3-46F2-A251-685A6604C56D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D2B234C-9E9E-4EEB-B630-07384D24E675}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5449,7 +5443,7 @@
         <xdr:cNvPr id="78" name="Рисунок 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CBB7E4C-A818-4A88-AAAD-369586F95855}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{023AA0C4-A9B6-48A7-A6E5-63FA903A6C2D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5499,7 +5493,7 @@
         <xdr:cNvPr id="79" name="Рисунок 78">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FD3B7C4-5F58-4F63-AA88-856FB98426AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E2D79F2-D008-4FB9-86B9-5DE424AA2A1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5549,7 +5543,7 @@
         <xdr:cNvPr id="80" name="Рисунок 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC0B9DB-D228-4679-AF70-77AA74BF0C69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C174D28-85F8-417B-9A53-BAD756711AED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5599,7 +5593,7 @@
         <xdr:cNvPr id="81" name="Рисунок 80">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E22D4B66-7D19-458B-BB86-95C21826A8DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A162FD2-B6D2-41E6-92E8-6A896407336B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5649,7 +5643,7 @@
         <xdr:cNvPr id="82" name="Рисунок 81">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DAE7091-E540-4E61-9C5B-16C679713215}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C4B08C8-48A2-4D8F-8EF3-860FB6D20225}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5699,7 +5693,7 @@
         <xdr:cNvPr id="83" name="Рисунок 82">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F847F8D-2558-4324-A46D-DDEEF4BB1E01}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{158A6379-049C-4F00-A1EA-C2B863EA5239}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5749,7 +5743,7 @@
         <xdr:cNvPr id="84" name="Рисунок 83">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC2347DA-E0C1-49E6-BA8B-6C36394E669F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A45ADE3-DB8E-4193-AE4F-13EC045CE036}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5799,7 +5793,7 @@
         <xdr:cNvPr id="85" name="Рисунок 84">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D463436-934D-4261-A333-AD95CA7478FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47CDC64A-D53D-4433-B98D-1B05BE5E4455}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5849,7 +5843,7 @@
         <xdr:cNvPr id="86" name="Рисунок 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6492E5B-488D-4111-85B1-542F09C5A1F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B075F33-5ED6-402F-A6B3-5CF83D6260B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5899,7 +5893,7 @@
         <xdr:cNvPr id="87" name="Рисунок 86">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F18EB52-4247-42AF-9E9E-8282B435CF60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFA88AA-A57F-45BB-BBA5-FE04CD1AA485}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5949,7 +5943,7 @@
         <xdr:cNvPr id="88" name="Рисунок 87">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30349403-D4C5-4413-BB3C-B8AD0DB77F15}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECB552E0-9C46-46B7-A9D3-52E9ABDE121F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5999,7 +5993,7 @@
         <xdr:cNvPr id="89" name="Рисунок 88">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711C4FED-34B4-43AF-8A30-AF033C2DC47F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{626FE9F2-E3A0-4932-B970-4AB3CC7D0AC6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6049,7 +6043,7 @@
         <xdr:cNvPr id="90" name="Рисунок 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25B6F8AC-ECE2-4D06-8A4E-1E208272EBD9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB1806F5-38DC-4A65-A6A1-0144D57BC03B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6099,7 +6093,7 @@
         <xdr:cNvPr id="91" name="Рисунок 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EC65224-C5E5-416F-8ADE-9643D62C4CEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8559F040-A545-4213-8D3F-35732D64CCBF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6149,7 +6143,7 @@
         <xdr:cNvPr id="92" name="Рисунок 91">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98E535FA-24AA-4929-AE83-96A8FF3C40A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9C5B1CD-7D32-4DC4-AC73-696CEA1340E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6199,7 +6193,7 @@
         <xdr:cNvPr id="93" name="Рисунок 92">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116A59AF-D373-42F1-9350-23AE44D53B8D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{286D396F-B236-4025-8A65-5AAC2F5333C7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6249,7 +6243,7 @@
         <xdr:cNvPr id="94" name="Рисунок 93">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4381AADC-B7CC-4224-A7E6-A8CD037683BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3836AA75-0DC8-47D4-98D7-7B75C013F6B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6299,7 +6293,7 @@
         <xdr:cNvPr id="95" name="Рисунок 94">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9FBE5B9-BB9A-4F84-B6D4-C076D0F5582C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A754C24B-C098-4B89-A3D4-FFBD75E2E295}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6349,7 +6343,7 @@
         <xdr:cNvPr id="96" name="Рисунок 95">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B5372A9-50FA-4938-9506-81903A8E4655}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B4F3C9B-21C2-4C4D-BC2B-2B7A7B94ECD8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6399,7 +6393,7 @@
         <xdr:cNvPr id="97" name="Рисунок 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5A64D99-A2B7-429B-899C-C97C6135A9B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EDCF25C-5A8F-442D-8671-5DDBC7BC9184}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6449,7 +6443,7 @@
         <xdr:cNvPr id="98" name="Рисунок 97">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAEE1EB-496C-4EE1-847C-B8A94330D10F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE02D600-E2D8-437F-8F37-E5371F79DA27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6499,7 +6493,7 @@
         <xdr:cNvPr id="99" name="Рисунок 98">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28873A79-E2F1-4792-9AFC-C288BBF50021}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86EF234A-EEA1-4826-8A88-1D3891DF5F66}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6549,7 +6543,7 @@
         <xdr:cNvPr id="100" name="Рисунок 99">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96E9B441-7F8A-405A-A995-9A4716CEA8BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5318167-2400-4475-BDC9-CEAF183002E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6599,7 +6593,7 @@
         <xdr:cNvPr id="101" name="Рисунок 100">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D4B55E0-F82E-41EB-8137-20E32ACE4BCB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEE3F8CC-B7FF-430E-AB9A-6A2D22299D6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6649,7 +6643,7 @@
         <xdr:cNvPr id="102" name="Рисунок 101">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5106E160-3EC7-487F-9170-D9470AEE40DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98B4CAF-318E-4B0D-A37A-DC765461DFB5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6699,7 +6693,7 @@
         <xdr:cNvPr id="103" name="Рисунок 102">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3F7C02-F703-4814-8D19-38628237C52B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80EF41FF-4DDE-4810-B390-48A1D4352C19}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6749,7 +6743,7 @@
         <xdr:cNvPr id="104" name="Рисунок 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48426BC5-C5D5-4D64-B079-3CD87377EC06}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0DE7FDD-8452-4DB1-AA99-94B3917CE76A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6799,7 +6793,7 @@
         <xdr:cNvPr id="105" name="Рисунок 104">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6100CCC8-EED6-4F34-A312-4C05AFC899FF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{659FBEAD-0B2D-4F2D-BE0B-E15FD77ED2BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6842,14 +6836,14 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1889125</xdr:colOff>
       <xdr:row>110</xdr:row>
-      <xdr:rowOff>1635713</xdr:rowOff>
+      <xdr:rowOff>1633565</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="106" name="Рисунок 105">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6698EBC7-F61D-4C00-8140-A25AC69F82CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E149D496-D48B-4589-A8BA-001013CBACDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6872,7 +6866,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4159250" y="157184142"/>
-          <a:ext cx="1778000" cy="1614071"/>
+          <a:ext cx="1778000" cy="1611923"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6899,7 +6893,7 @@
         <xdr:cNvPr id="107" name="Рисунок 106">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F94F9AB0-D9D1-43C0-B44F-BB97ADEC2582}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85A81FA7-E05A-47B4-996F-B16DB5AF9251}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6949,7 +6943,7 @@
         <xdr:cNvPr id="108" name="Рисунок 107">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{817F7207-9F4F-4E51-B9E1-12DB630EC6CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A739C050-59A1-4953-8689-E71C4692E6F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6999,7 +6993,7 @@
         <xdr:cNvPr id="109" name="Рисунок 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D03C45B5-7592-4107-B927-BFDE085A38A8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{334EC93E-13C8-4CDD-AC69-B93E63AD2DE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7049,7 +7043,7 @@
         <xdr:cNvPr id="110" name="Рисунок 109">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2E9C904-3E05-403D-B781-19BDE88FB95C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{587E739B-B618-488E-8851-9C09788727C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7099,7 +7093,7 @@
         <xdr:cNvPr id="111" name="Рисунок 110">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{158D39B2-DD5C-49D9-B22E-9BC74C4E490A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D5F82AD-57A7-4233-A749-99FA614380A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7149,7 +7143,7 @@
         <xdr:cNvPr id="112" name="Рисунок 111">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACADF2BF-6E18-48AB-B801-ADACB215BE7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE041B98-F5B8-42F2-ACCD-9AF438842039}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7199,7 +7193,7 @@
         <xdr:cNvPr id="113" name="Рисунок 112">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FD8D2D5-1FAE-4B78-B701-DA9B986050E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3003F0E5-2FFB-4627-8BF8-A34C34D6137C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7249,7 +7243,7 @@
         <xdr:cNvPr id="114" name="Рисунок 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E433981-CB02-4591-A395-BE27F08DF708}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58341020-D298-40A1-9249-855469FC201D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7299,7 +7293,7 @@
         <xdr:cNvPr id="115" name="Рисунок 114">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72FF67A3-16A6-440E-8AFD-AFF02A56E2BD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94D1A75D-6B69-4B3F-9EC8-B366A76307E0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7349,7 +7343,7 @@
         <xdr:cNvPr id="116" name="Рисунок 115">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{981FF25F-EB7D-4105-8225-29D62AAB5C6D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C3F451F-0FF3-410D-8CE7-F0C81D601127}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7399,7 +7393,7 @@
         <xdr:cNvPr id="117" name="Рисунок 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B09CA90-3996-4B28-ABAC-B38A43DFB059}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67A66F4E-5635-47DA-B3DF-3C7946092DC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7449,7 +7443,7 @@
         <xdr:cNvPr id="118" name="Рисунок 117">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB0DF919-6251-4B29-9ED3-0A4CA09C6E0F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FDDE907-9242-4649-A3F8-038E99BA00C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7499,7 +7493,7 @@
         <xdr:cNvPr id="119" name="Рисунок 118">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{405B9BF0-D148-44D5-B4D6-ED8E610807BF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBC35D37-FB50-4B10-9373-8E23C4663A3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7549,7 +7543,7 @@
         <xdr:cNvPr id="120" name="Рисунок 119">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E53045B6-A319-4929-B7FD-835C50ABD890}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{034A6209-9413-4931-B211-4A46E6EE306D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7599,7 +7593,7 @@
         <xdr:cNvPr id="121" name="Рисунок 120">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78C3BFC9-45FF-43A7-9E71-13A9FBA1AD31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA767B2B-AEA2-49C6-BE3E-F3D7A4800368}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7649,7 +7643,7 @@
         <xdr:cNvPr id="122" name="Рисунок 121">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FABF0D7-BE07-4B9A-A30A-3C0ADA610320}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6C78975-7F42-46C3-86BD-8964DFEEA035}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7699,7 +7693,7 @@
         <xdr:cNvPr id="123" name="Рисунок 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DF265FE-7406-46EB-983B-B9FC037931EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8E25ACE-C360-4901-94EA-598E5E1E1526}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7749,7 +7743,7 @@
         <xdr:cNvPr id="124" name="Рисунок 123">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91CEC514-9BB0-4522-9224-E8719F6BBF19}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67FEDB2E-B880-4A34-9FED-60D6E18629FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7799,7 +7793,7 @@
         <xdr:cNvPr id="125" name="Рисунок 124">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4AD69A7-C7E1-4DFC-8A67-08CA5218F284}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4593B8B0-7DE4-48D5-9B5C-935BB20094F1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7849,7 +7843,7 @@
         <xdr:cNvPr id="126" name="Рисунок 125">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACFC67B-FB33-4D4B-B9E8-DF38AC81C478}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9FBA3A7-8699-4E5E-86B8-075654043A05}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7899,7 +7893,7 @@
         <xdr:cNvPr id="127" name="Рисунок 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E903E0E-3868-4DF9-BD6A-51F7C07B56BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFFC401A-017F-4F68-B052-03EEB33E47A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7949,7 +7943,7 @@
         <xdr:cNvPr id="128" name="Рисунок 127">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39D54D70-5E93-42CF-BBEC-A1C61111A391}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1179D7D2-FD52-4E24-8C27-7A672967DB0D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7999,7 +7993,7 @@
         <xdr:cNvPr id="129" name="Рисунок 128">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E3AAEBA-602C-4211-A4F8-9813E8B420CC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{790B8486-CDCE-476F-A45D-C1B390EAF26D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8049,7 +8043,7 @@
         <xdr:cNvPr id="130" name="Рисунок 129">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D8995B9-4379-4C62-93B3-86E438E2D823}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE4D43FD-ED56-4A45-A8DD-304EBA6531EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8099,7 +8093,7 @@
         <xdr:cNvPr id="131" name="Рисунок 130">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4F60031-277A-457C-B209-C18568619745}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C3625F7-A745-4FA0-A892-4DD851B55684}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8149,7 +8143,7 @@
         <xdr:cNvPr id="132" name="Рисунок 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F698F84-5FBB-4EDE-B497-0DEEA900A7E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5B8DDB8-5982-41D6-BAA6-3700B0EED90E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8199,7 +8193,7 @@
         <xdr:cNvPr id="133" name="Рисунок 132">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{459AEC5B-99AD-49A6-9794-F7EDF42810AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BEB560B-F6DB-4C9A-8A42-8ACD186587B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8249,7 +8243,7 @@
         <xdr:cNvPr id="134" name="Рисунок 133">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82019306-AE1A-4062-8DBF-0504A6F6809A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D27A54-949C-4A7E-9B0C-6820B51C34EB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8299,7 +8293,7 @@
         <xdr:cNvPr id="135" name="Рисунок 134">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F79A1E3B-72C4-4A1B-B545-63AEDB1E17BB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B414B7C2-1B59-49D6-84E5-7895DC46FE33}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8349,7 +8343,7 @@
         <xdr:cNvPr id="136" name="Рисунок 135">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B607098-DA7F-4880-B5F3-65C9316E5165}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DCB46DF-1879-4405-A450-2267CD5966F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8399,7 +8393,7 @@
         <xdr:cNvPr id="137" name="Рисунок 136">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{522960AB-0402-488A-9B58-CACD7C93FB39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D89040F5-5873-42BF-8341-8C8A44C5CA52}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8449,7 +8443,7 @@
         <xdr:cNvPr id="138" name="Рисунок 137">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90D12E5D-07F9-4DEC-9537-B879424098D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49A77306-7561-43AA-820E-7B592F62D680}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8499,7 +8493,7 @@
         <xdr:cNvPr id="139" name="Рисунок 138">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26A1D788-0131-4BBB-85F3-CC95D94E2CA3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C55C87D-A8DE-4332-B5AE-8672DFF5EA1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8549,7 +8543,7 @@
         <xdr:cNvPr id="140" name="Рисунок 139">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6600CAED-91E1-4175-80F7-EC9FED6FDDBF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA89795-E450-4C30-92AD-A9866EBBECCA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8599,7 +8593,7 @@
         <xdr:cNvPr id="141" name="Рисунок 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{848339F5-ABB4-4A4B-A018-2CB92283CC43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD6F85B9-7856-4868-94AB-1ADBAB10A308}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8649,7 +8643,7 @@
         <xdr:cNvPr id="142" name="Рисунок 141">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57C82613-E830-4EEE-9856-0A705A326F90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6366CD14-F7EC-4F5C-9148-F74E04A908C5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8699,7 +8693,7 @@
         <xdr:cNvPr id="143" name="Рисунок 142">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B84E02F5-2EFB-48FB-9D35-DE0244996529}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5608EBF9-5A96-45A5-8156-E9CFDD1EB7F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8749,7 +8743,7 @@
         <xdr:cNvPr id="144" name="Рисунок 143">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47AC00E4-F3FA-46F8-B142-A1E9CA7C863F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ECDC6A95-332D-47CD-9384-38B4E9AC7E10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8799,7 +8793,7 @@
         <xdr:cNvPr id="145" name="Рисунок 144">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0689D3F-15B7-46EE-9041-EDCB4CE9F297}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D82031F3-A139-42E8-8062-EC2CAEFB94C8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8849,7 +8843,7 @@
         <xdr:cNvPr id="146" name="Рисунок 145">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD94AC3E-E7F2-4E64-8691-45BE910F8F29}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B8C52A9-45FA-4BE6-87DE-414B6C03D0F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8899,7 +8893,7 @@
         <xdr:cNvPr id="147" name="Рисунок 146">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE441505-8024-4C7B-930C-8BB2E698737F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9134F48-7E4B-42CE-99DC-4C553CF86736}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8949,7 +8943,7 @@
         <xdr:cNvPr id="148" name="Рисунок 147">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8BE981C-7FD1-4435-A3D9-D4A7E073A2A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09457107-C651-46ED-85C0-B279D0C94D0C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8999,7 +8993,7 @@
         <xdr:cNvPr id="149" name="Рисунок 148">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC67EF2E-296A-4B59-82A9-09BCD4ED712B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FBD64AD-5449-4AE6-8504-3DE2DA9A68AE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9049,7 +9043,7 @@
         <xdr:cNvPr id="150" name="Рисунок 149">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B60383BE-D5EE-490F-8839-67E5845C9CF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5340A296-9064-44A4-8F67-A5E7DCB090D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9099,7 +9093,7 @@
         <xdr:cNvPr id="151" name="Рисунок 150">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{978D8A4C-DCAE-4B6E-A3F0-098770FDAB0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE32191F-8FBC-4FE9-9363-F6214BBBED18}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9149,7 +9143,7 @@
         <xdr:cNvPr id="152" name="Рисунок 151">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0AC3A3E-2140-4718-9209-D487E3E0D48D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA6A3C55-F68A-46D7-851F-65F548C8EE54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9199,7 +9193,7 @@
         <xdr:cNvPr id="153" name="Рисунок 152">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C52BBEB5-3EB6-461D-9CEC-CAB57BD276AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37892252-1D2E-45C5-A14D-7F9E4AD972A5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9249,7 +9243,7 @@
         <xdr:cNvPr id="154" name="Рисунок 153">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBC3E89C-574C-4632-9D61-620178380C47}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35DD288C-6EE0-4DEB-880E-154C49226233}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9299,7 +9293,7 @@
         <xdr:cNvPr id="155" name="Рисунок 154">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA162D8D-7D33-4D67-A9FB-DE24E3BEF9FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CC99FA7-CC73-49D9-95BD-FBC690AB42D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9349,7 +9343,7 @@
         <xdr:cNvPr id="156" name="Рисунок 155">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A5030DE-A2D9-4D1F-AAC3-8A2BF4B051AD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9375F09-ABA3-4140-8922-110CA30E2157}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9399,7 +9393,7 @@
         <xdr:cNvPr id="157" name="Рисунок 156">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3266E50-FA48-4CAB-BC78-988D9378891C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6DC648-EDE9-4D54-8CE6-4389CAA9C88A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9449,7 +9443,7 @@
         <xdr:cNvPr id="158" name="Рисунок 157">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7C7A3DF2-D89E-4DD1-9AB4-82CFC3FE45A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DC955E9-9A2D-436F-9E5F-ADF884CB36C0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9499,7 +9493,7 @@
         <xdr:cNvPr id="159" name="Рисунок 158">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE7466DC-08C0-4D1E-B9AA-757F28EBA96C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51BA63C9-AB2F-40A3-BD0E-B7DF4D3A5C78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9549,7 +9543,7 @@
         <xdr:cNvPr id="160" name="Рисунок 159">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6916CB58-D8E1-475D-A81B-5EEB618EE4F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6FCAA57-A608-4CDE-B48A-930EECE2B91C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9599,7 +9593,7 @@
         <xdr:cNvPr id="161" name="Рисунок 160">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A6F8BDF0-3FB3-437E-B989-E9F81BC368FB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48695D53-4390-472B-838D-50C9E8FF2BA5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9649,7 +9643,7 @@
         <xdr:cNvPr id="162" name="Рисунок 161">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5387E612-5856-4CD1-B083-797B778788A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11CDA190-7911-48D4-AEF5-12D6179E0A78}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9699,7 +9693,7 @@
         <xdr:cNvPr id="163" name="Рисунок 162">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DC2F7303-5706-451A-98DA-7E581A484692}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D0E9CAA-902D-4BD9-9AF1-5E8B6DA6A2C6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9749,7 +9743,7 @@
         <xdr:cNvPr id="164" name="Рисунок 163">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB1C271A-C6C3-4A0E-9F2E-7BCE8EF107DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5CB995A-4780-4A10-9385-6472B347B598}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9799,7 +9793,7 @@
         <xdr:cNvPr id="165" name="Рисунок 164">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97DFDC11-BC2D-49C5-BF48-6375CCA2ABD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B396522E-60E0-4682-A26A-2EC358DE5A50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9849,7 +9843,7 @@
         <xdr:cNvPr id="166" name="Рисунок 165">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC935549-D335-4262-8569-109F6C5C73DA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C92746-FC60-4C77-9661-3BD9ABF347C3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9899,7 +9893,7 @@
         <xdr:cNvPr id="167" name="Рисунок 166">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82485772-0B84-4C49-B3A8-2C4D431CC353}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{281085FA-C133-4584-83C0-12FD409F4D3E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9949,7 +9943,7 @@
         <xdr:cNvPr id="168" name="Рисунок 167">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B7A81A5-1F56-459C-8C82-24A68EEEA75B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C859A085-B325-404C-9E7C-3F75E47B71BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9999,7 +9993,7 @@
         <xdr:cNvPr id="169" name="Рисунок 168">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35C8E443-E288-4881-AAE4-9331416C0BF4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3C39F3-912F-4748-BF3E-CB06BB94D6E2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10049,7 +10043,7 @@
         <xdr:cNvPr id="170" name="Рисунок 169">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{774BA718-E4FA-4E03-9D57-9DC9129DDA1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92C0C06C-6546-4FD5-93FB-EBD8E8FB81F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10380,14 +10374,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2CB3F3-5B1C-4C28-8D75-6CAC814E09ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7EB2F3-8F12-4A17-AE2B-1C75103D7E0F}">
   <sheetPr codeName="Лист9">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:BG172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="BF1" sqref="BF1:BF1048576"/>
     </sheetView>
   </sheetViews>
@@ -19333,10 +19327,10 @@
         <v>120</v>
       </c>
       <c r="K104" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="L104" s="31" t="s">
         <v>290</v>
-      </c>
-      <c r="L104" s="20" t="s">
-        <v>47</v>
       </c>
       <c r="M104" s="13" t="s">
         <v>48</v>
@@ -19418,10 +19412,10 @@
       <c r="J105" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="K105" s="29" t="s">
-        <v>293</v>
-      </c>
-      <c r="L105" s="20" t="s">
+      <c r="K105" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="L105" s="31" t="s">
         <v>47</v>
       </c>
       <c r="M105" s="13" t="s">
@@ -19479,10 +19473,10 @@
     </row>
     <row r="106" spans="1:38" s="28" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="12" t="s">
+        <v>293</v>
+      </c>
+      <c r="B106" s="13" t="s">
         <v>294</v>
-      </c>
-      <c r="B106" s="13" t="s">
-        <v>295</v>
       </c>
       <c r="C106" s="13"/>
       <c r="D106" s="14" t="s">
@@ -19508,7 +19502,7 @@
         <v>83</v>
       </c>
       <c r="L106" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M106" s="13" t="s">
         <v>48</v>
@@ -19565,10 +19559,10 @@
     </row>
     <row r="107" spans="1:38" s="28" customFormat="1" ht="121.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B107" s="13" t="s">
         <v>297</v>
-      </c>
-      <c r="B107" s="13" t="s">
-        <v>298</v>
       </c>
       <c r="C107" s="13"/>
       <c r="D107" s="14" t="s">
@@ -19594,7 +19588,7 @@
         <v>83</v>
       </c>
       <c r="L107" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M107" s="13" t="s">
         <v>48</v>
@@ -19651,10 +19645,10 @@
     </row>
     <row r="108" spans="1:38" s="28" customFormat="1" ht="124.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="B108" s="13" t="s">
         <v>299</v>
-      </c>
-      <c r="B108" s="13" t="s">
-        <v>300</v>
       </c>
       <c r="C108" s="13"/>
       <c r="D108" s="14" t="s">
@@ -19680,7 +19674,7 @@
         <v>83</v>
       </c>
       <c r="L108" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M108" s="13" t="s">
         <v>48</v>
@@ -19737,10 +19731,10 @@
     </row>
     <row r="109" spans="1:38" s="28" customFormat="1" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
+        <v>300</v>
+      </c>
+      <c r="B109" s="13" t="s">
         <v>301</v>
-      </c>
-      <c r="B109" s="13" t="s">
-        <v>302</v>
       </c>
       <c r="C109" s="13"/>
       <c r="D109" s="14" t="s">
@@ -19766,7 +19760,7 @@
         <v>83</v>
       </c>
       <c r="L109" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M109" s="13" t="s">
         <v>48</v>
@@ -19823,10 +19817,10 @@
     </row>
     <row r="110" spans="1:38" s="28" customFormat="1" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="B110" s="13" t="s">
         <v>303</v>
-      </c>
-      <c r="B110" s="13" t="s">
-        <v>304</v>
       </c>
       <c r="C110" s="13"/>
       <c r="D110" s="14" t="s">
@@ -19846,13 +19840,13 @@
         <v>44</v>
       </c>
       <c r="J110" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="K110" s="29" t="s">
         <v>305</v>
       </c>
-      <c r="K110" s="29" t="s">
-        <v>306</v>
-      </c>
       <c r="L110" s="20" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="M110" s="13" t="s">
         <v>48</v>
@@ -19909,10 +19903,10 @@
     </row>
     <row r="111" spans="1:38" s="28" customFormat="1" ht="131.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C111" s="13"/>
       <c r="D111" s="14" t="s">
@@ -19932,13 +19926,13 @@
         <v>44</v>
       </c>
       <c r="J111" s="26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K111" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L111" s="20" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="M111" s="13" t="s">
         <v>48</v>
@@ -19995,10 +19989,10 @@
     </row>
     <row r="112" spans="1:38" s="28" customFormat="1" ht="123.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C112" s="13"/>
       <c r="D112" s="14" t="s">
@@ -20024,7 +20018,7 @@
         <v>137</v>
       </c>
       <c r="L112" s="20" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="M112" s="13" t="s">
         <v>48</v>
@@ -20081,10 +20075,10 @@
     </row>
     <row r="113" spans="1:38" s="28" customFormat="1" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C113" s="13"/>
       <c r="D113" s="14" t="s">
@@ -20110,7 +20104,7 @@
         <v>83</v>
       </c>
       <c r="L113" s="20" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="M113" s="13" t="s">
         <v>48</v>
@@ -20167,10 +20161,10 @@
     </row>
     <row r="114" spans="1:38" s="28" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="12" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C114" s="13"/>
       <c r="D114" s="14" t="s">
@@ -20196,7 +20190,7 @@
         <v>83</v>
       </c>
       <c r="L114" s="20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M114" s="13" t="s">
         <v>48</v>
@@ -20253,10 +20247,10 @@
     </row>
     <row r="115" spans="1:38" s="28" customFormat="1" ht="124.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C115" s="13"/>
       <c r="D115" s="14" t="s">
@@ -20279,10 +20273,10 @@
         <v>63</v>
       </c>
       <c r="K115" s="29" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="L115" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M115" s="13" t="s">
         <v>48</v>
@@ -20339,10 +20333,10 @@
     </row>
     <row r="116" spans="1:38" s="28" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="12" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C116" s="13"/>
       <c r="D116" s="14" t="s">
@@ -20365,10 +20359,10 @@
         <v>142</v>
       </c>
       <c r="K116" s="29" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L116" s="20" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M116" s="13" t="s">
         <v>48</v>
@@ -20425,10 +20419,10 @@
     </row>
     <row r="117" spans="1:38" s="28" customFormat="1" ht="120.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C117" s="13"/>
       <c r="D117" s="14" t="s">
@@ -20451,10 +20445,10 @@
         <v>55</v>
       </c>
       <c r="K117" s="27" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L117" s="20" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="M117" s="13" t="s">
         <v>48</v>
@@ -20511,7 +20505,7 @@
     </row>
     <row r="118" spans="1:38" s="28" customFormat="1" ht="127.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="12" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B118" s="13" t="s">
         <v>105</v>
@@ -20537,10 +20531,10 @@
         <v>159</v>
       </c>
       <c r="K118" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L118" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M118" s="13" t="s">
         <v>48</v>
@@ -20597,7 +20591,7 @@
     </row>
     <row r="119" spans="1:38" s="28" customFormat="1" ht="122.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B119" s="13" t="s">
         <v>148</v>
@@ -20623,10 +20617,10 @@
         <v>159</v>
       </c>
       <c r="K119" s="27" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="L119" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M119" s="13" t="s">
         <v>48</v>
@@ -20683,10 +20677,10 @@
     </row>
     <row r="120" spans="1:38" s="28" customFormat="1" ht="125.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="12" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C120" s="13"/>
       <c r="D120" s="14" t="s">
@@ -20712,7 +20706,7 @@
         <v>83</v>
       </c>
       <c r="L120" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M120" s="13" t="s">
         <v>48</v>
@@ -20769,10 +20763,10 @@
     </row>
     <row r="121" spans="1:38" s="28" customFormat="1" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C121" s="13"/>
       <c r="D121" s="14" t="s">
@@ -20798,7 +20792,7 @@
         <v>98</v>
       </c>
       <c r="L121" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M121" s="13" t="s">
         <v>48</v>
@@ -20855,10 +20849,10 @@
     </row>
     <row r="122" spans="1:38" s="28" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="12" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C122" s="13"/>
       <c r="D122" s="14" t="s">
@@ -20878,13 +20872,13 @@
         <v>44</v>
       </c>
       <c r="J122" s="26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K122" s="29" t="s">
         <v>222</v>
       </c>
       <c r="L122" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M122" s="13" t="s">
         <v>48</v>
@@ -20941,10 +20935,10 @@
     </row>
     <row r="123" spans="1:38" s="28" customFormat="1" ht="127.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C123" s="13"/>
       <c r="D123" s="14" t="s">
@@ -20967,10 +20961,10 @@
         <v>120</v>
       </c>
       <c r="K123" s="27" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="L123" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M123" s="13" t="s">
         <v>48</v>
@@ -21027,10 +21021,10 @@
     </row>
     <row r="124" spans="1:38" s="28" customFormat="1" ht="121.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="12" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C124" s="13"/>
       <c r="D124" s="14" t="s">
@@ -21056,7 +21050,7 @@
         <v>98</v>
       </c>
       <c r="L124" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M124" s="13" t="s">
         <v>48</v>
@@ -21113,10 +21107,10 @@
     </row>
     <row r="125" spans="1:38" s="28" customFormat="1" ht="130.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C125" s="13"/>
       <c r="D125" s="14" t="s">
@@ -21136,13 +21130,13 @@
         <v>44</v>
       </c>
       <c r="J125" s="26" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="K125" s="27" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L125" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M125" s="13" t="s">
         <v>48</v>
@@ -21199,10 +21193,10 @@
     </row>
     <row r="126" spans="1:38" s="28" customFormat="1" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C126" s="13"/>
       <c r="D126" s="14" t="s">
@@ -21228,7 +21222,7 @@
         <v>60</v>
       </c>
       <c r="L126" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M126" s="13" t="s">
         <v>48</v>
@@ -21285,10 +21279,10 @@
     </row>
     <row r="127" spans="1:38" s="28" customFormat="1" ht="122.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C127" s="13"/>
       <c r="D127" s="14" t="s">
@@ -21314,7 +21308,7 @@
         <v>137</v>
       </c>
       <c r="L127" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M127" s="13" t="s">
         <v>48</v>
@@ -21371,10 +21365,10 @@
     </row>
     <row r="128" spans="1:38" s="28" customFormat="1" ht="113.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C128" s="13"/>
       <c r="D128" s="14" t="s">
@@ -21397,10 +21391,10 @@
         <v>59</v>
       </c>
       <c r="K128" s="29" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L128" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M128" s="13" t="s">
         <v>48</v>
@@ -21457,10 +21451,10 @@
     </row>
     <row r="129" spans="1:38" s="28" customFormat="1" ht="124.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C129" s="13"/>
       <c r="D129" s="14" t="s">
@@ -21486,7 +21480,7 @@
         <v>83</v>
       </c>
       <c r="L129" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M129" s="13" t="s">
         <v>48</v>
@@ -21543,10 +21537,10 @@
     </row>
     <row r="130" spans="1:38" s="28" customFormat="1" ht="125.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C130" s="13"/>
       <c r="D130" s="14" t="s">
@@ -21572,7 +21566,7 @@
         <v>108</v>
       </c>
       <c r="L130" s="15" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="M130" s="13" t="s">
         <v>48</v>
@@ -21629,10 +21623,10 @@
     </row>
     <row r="131" spans="1:38" s="28" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C131" s="13"/>
       <c r="D131" s="14" t="s">
@@ -21652,13 +21646,13 @@
         <v>44</v>
       </c>
       <c r="J131" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K131" s="27" t="s">
         <v>264</v>
       </c>
       <c r="L131" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M131" s="13" t="s">
         <v>48</v>
@@ -21715,10 +21709,10 @@
     </row>
     <row r="132" spans="1:38" s="28" customFormat="1" ht="123.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="12" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C132" s="13"/>
       <c r="D132" s="14" t="s">
@@ -21744,7 +21738,7 @@
         <v>83</v>
       </c>
       <c r="L132" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M132" s="13" t="s">
         <v>48</v>
@@ -21801,10 +21795,10 @@
     </row>
     <row r="133" spans="1:38" s="28" customFormat="1" ht="119.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C133" s="13"/>
       <c r="D133" s="14" t="s">
@@ -21830,7 +21824,7 @@
         <v>98</v>
       </c>
       <c r="L133" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M133" s="13" t="s">
         <v>48</v>
@@ -21887,7 +21881,7 @@
     </row>
     <row r="134" spans="1:38" s="28" customFormat="1" ht="129.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="12" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B134" s="13" t="s">
         <v>258</v>
@@ -21916,7 +21910,7 @@
         <v>98</v>
       </c>
       <c r="L134" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M134" s="13" t="s">
         <v>48</v>
@@ -21973,10 +21967,10 @@
     </row>
     <row r="135" spans="1:38" s="28" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C135" s="13"/>
       <c r="D135" s="14" t="s">
@@ -22002,7 +21996,7 @@
         <v>137</v>
       </c>
       <c r="L135" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M135" s="13" t="s">
         <v>48</v>
@@ -22059,10 +22053,10 @@
     </row>
     <row r="136" spans="1:38" s="28" customFormat="1" ht="114.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C136" s="13"/>
       <c r="D136" s="14" t="s">
@@ -22088,7 +22082,7 @@
         <v>137</v>
       </c>
       <c r="L136" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M136" s="13" t="s">
         <v>48</v>
@@ -22145,7 +22139,7 @@
     </row>
     <row r="137" spans="1:38" s="28" customFormat="1" ht="115.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B137" s="13" t="s">
         <v>240</v>
@@ -22174,7 +22168,7 @@
         <v>123</v>
       </c>
       <c r="L137" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M137" s="13" t="s">
         <v>48</v>
@@ -22231,10 +22225,10 @@
     </row>
     <row r="138" spans="1:38" s="28" customFormat="1" ht="122.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C138" s="13"/>
       <c r="D138" s="14" t="s">
@@ -22260,7 +22254,7 @@
         <v>83</v>
       </c>
       <c r="L138" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M138" s="13" t="s">
         <v>48</v>
@@ -22317,10 +22311,10 @@
     </row>
     <row r="139" spans="1:38" s="28" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C139" s="13"/>
       <c r="D139" s="14" t="s">
@@ -22346,7 +22340,7 @@
         <v>83</v>
       </c>
       <c r="L139" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M139" s="13" t="s">
         <v>48</v>
@@ -22403,10 +22397,10 @@
     </row>
     <row r="140" spans="1:38" s="28" customFormat="1" ht="124.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="12" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C140" s="13"/>
       <c r="D140" s="14" t="s">
@@ -22429,10 +22423,10 @@
         <v>67</v>
       </c>
       <c r="K140" s="27" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="L140" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M140" s="13" t="s">
         <v>48</v>
@@ -22489,10 +22483,10 @@
     </row>
     <row r="141" spans="1:38" s="28" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C141" s="13"/>
       <c r="D141" s="14" t="s">
@@ -22512,13 +22506,13 @@
         <v>44</v>
       </c>
       <c r="J141" s="26" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="K141" s="27" t="s">
         <v>264</v>
       </c>
       <c r="L141" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M141" s="13" t="s">
         <v>48</v>
@@ -22575,23 +22569,23 @@
     </row>
     <row r="142" spans="1:38" s="28" customFormat="1" ht="135.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C142" s="13"/>
       <c r="D142" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E142" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F142" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G142" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H142" s="13"/>
       <c r="I142" s="14" t="s">
@@ -22604,10 +22598,10 @@
         <v>83</v>
       </c>
       <c r="L142" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M142" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N142" s="14" t="s">
         <v>49</v>
@@ -22661,23 +22655,23 @@
     </row>
     <row r="143" spans="1:38" s="28" customFormat="1" ht="141.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C143" s="13"/>
       <c r="D143" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F143" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G143" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H143" s="13"/>
       <c r="I143" s="14" t="s">
@@ -22687,13 +22681,13 @@
         <v>159</v>
       </c>
       <c r="K143" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L143" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M143" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N143" s="14" t="s">
         <v>49</v>
@@ -22747,39 +22741,39 @@
     </row>
     <row r="144" spans="1:38" s="28" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C144" s="13"/>
       <c r="D144" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E144" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F144" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G144" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H144" s="13"/>
       <c r="I144" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J144" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K144" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L144" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M144" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N144" s="14" t="s">
         <v>49</v>
@@ -22833,23 +22827,23 @@
     </row>
     <row r="145" spans="1:38" s="28" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C145" s="13"/>
       <c r="D145" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E145" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F145" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G145" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H145" s="13"/>
       <c r="I145" s="14" t="s">
@@ -22859,13 +22853,13 @@
         <v>159</v>
       </c>
       <c r="K145" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L145" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M145" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N145" s="14" t="s">
         <v>49</v>
@@ -22919,39 +22913,39 @@
     </row>
     <row r="146" spans="1:38" s="28" customFormat="1" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="12" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C146" s="13"/>
       <c r="D146" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E146" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F146" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G146" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H146" s="13"/>
       <c r="I146" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J146" s="26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K146" s="27" t="s">
         <v>137</v>
       </c>
       <c r="L146" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M146" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N146" s="14" t="s">
         <v>49</v>
@@ -23005,23 +22999,23 @@
     </row>
     <row r="147" spans="1:38" s="28" customFormat="1" ht="133.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C147" s="13"/>
       <c r="D147" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E147" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F147" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G147" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H147" s="13"/>
       <c r="I147" s="14" t="s">
@@ -23034,10 +23028,10 @@
         <v>83</v>
       </c>
       <c r="L147" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M147" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N147" s="14" t="s">
         <v>49</v>
@@ -23091,23 +23085,23 @@
     </row>
     <row r="148" spans="1:38" s="28" customFormat="1" ht="129.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C148" s="13"/>
       <c r="D148" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E148" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F148" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G148" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H148" s="13"/>
       <c r="I148" s="14" t="s">
@@ -23120,10 +23114,10 @@
         <v>83</v>
       </c>
       <c r="L148" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M148" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N148" s="14" t="s">
         <v>49</v>
@@ -23177,23 +23171,23 @@
     </row>
     <row r="149" spans="1:38" s="28" customFormat="1" ht="139.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C149" s="13"/>
       <c r="D149" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E149" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F149" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G149" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H149" s="13"/>
       <c r="I149" s="14" t="s">
@@ -23206,10 +23200,10 @@
         <v>83</v>
       </c>
       <c r="L149" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M149" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N149" s="14" t="s">
         <v>49</v>
@@ -23263,23 +23257,23 @@
     </row>
     <row r="150" spans="1:38" s="28" customFormat="1" ht="130.69999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C150" s="13"/>
       <c r="D150" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E150" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F150" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G150" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H150" s="13"/>
       <c r="I150" s="14" t="s">
@@ -23292,10 +23286,10 @@
         <v>83</v>
       </c>
       <c r="L150" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M150" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N150" s="14" t="s">
         <v>49</v>
@@ -23349,23 +23343,23 @@
     </row>
     <row r="151" spans="1:38" s="28" customFormat="1" ht="137.85" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C151" s="13"/>
       <c r="D151" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E151" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F151" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G151" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H151" s="13"/>
       <c r="I151" s="14" t="s">
@@ -23378,10 +23372,10 @@
         <v>83</v>
       </c>
       <c r="L151" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M151" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N151" s="14" t="s">
         <v>49</v>
@@ -23435,39 +23429,39 @@
     </row>
     <row r="152" spans="1:38" s="28" customFormat="1" ht="133.69999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C152" s="13"/>
       <c r="D152" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E152" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F152" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G152" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H152" s="13"/>
       <c r="I152" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J152" s="26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="K152" s="27" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L152" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M152" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N152" s="14" t="s">
         <v>49</v>
@@ -23521,23 +23515,23 @@
     </row>
     <row r="153" spans="1:38" s="28" customFormat="1" ht="148.69999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B153" s="13" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C153" s="13"/>
       <c r="D153" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E153" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F153" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G153" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H153" s="13"/>
       <c r="I153" s="14" t="s">
@@ -23550,10 +23544,10 @@
         <v>60</v>
       </c>
       <c r="L153" s="31" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M153" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N153" s="14" t="s">
         <v>49</v>
@@ -23607,23 +23601,23 @@
     </row>
     <row r="154" spans="1:38" s="28" customFormat="1" ht="139.69999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="12" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B154" s="13" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C154" s="13"/>
       <c r="D154" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E154" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F154" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G154" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H154" s="13"/>
       <c r="I154" s="14" t="s">
@@ -23633,13 +23627,13 @@
         <v>159</v>
       </c>
       <c r="K154" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L154" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M154" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N154" s="14" t="s">
         <v>49</v>
@@ -23693,39 +23687,39 @@
     </row>
     <row r="155" spans="1:38" s="28" customFormat="1" ht="145.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B155" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C155" s="13"/>
       <c r="D155" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E155" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F155" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G155" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H155" s="13"/>
       <c r="I155" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J155" s="26" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="K155" s="27" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L155" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M155" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N155" s="14" t="s">
         <v>49</v>
@@ -23779,39 +23773,39 @@
     </row>
     <row r="156" spans="1:38" s="28" customFormat="1" ht="137.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="12" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B156" s="13" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C156" s="13"/>
       <c r="D156" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E156" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F156" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G156" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H156" s="13"/>
       <c r="I156" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J156" s="26" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="K156" s="27" t="s">
         <v>111</v>
       </c>
       <c r="L156" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M156" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N156" s="14" t="s">
         <v>49</v>
@@ -23865,39 +23859,39 @@
     </row>
     <row r="157" spans="1:38" s="28" customFormat="1" ht="142.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B157" s="13" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C157" s="13"/>
       <c r="D157" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E157" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F157" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G157" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H157" s="13"/>
       <c r="I157" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J157" s="26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K157" s="27" t="s">
         <v>137</v>
       </c>
       <c r="L157" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M157" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N157" s="14" t="s">
         <v>49</v>
@@ -23951,39 +23945,39 @@
     </row>
     <row r="158" spans="1:38" s="28" customFormat="1" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="12" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B158" s="13" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C158" s="13"/>
       <c r="D158" s="14" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E158" s="14" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F158" s="14" t="s">
         <v>42</v>
       </c>
       <c r="G158" s="14" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H158" s="13"/>
       <c r="I158" s="14" t="s">
         <v>44</v>
       </c>
       <c r="J158" s="26" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="K158" s="27" t="s">
         <v>83</v>
       </c>
       <c r="L158" s="20" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M158" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="N158" s="14" t="s">
         <v>49</v>
@@ -24037,10 +24031,10 @@
     </row>
     <row r="159" spans="1:38" s="28" customFormat="1" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B159" s="13" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C159" s="13"/>
       <c r="D159" s="14" t="s">
@@ -24066,7 +24060,7 @@
         <v>83</v>
       </c>
       <c r="L159" s="20" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="M159" s="13" t="s">
         <v>48</v>
@@ -24123,10 +24117,10 @@
     </row>
     <row r="160" spans="1:38" s="28" customFormat="1" ht="131.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B160" s="13" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C160" s="13"/>
       <c r="D160" s="14" t="s">
@@ -24146,13 +24140,13 @@
         <v>44</v>
       </c>
       <c r="J160" s="26" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="K160" s="27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L160" s="20" t="s">
-        <v>307</v>
+        <v>290</v>
       </c>
       <c r="M160" s="13" t="s">
         <v>48</v>
@@ -24209,10 +24203,10 @@
     </row>
     <row r="161" spans="1:38" s="28" customFormat="1" ht="121.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B161" s="13" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C161" s="13"/>
       <c r="D161" s="14" t="s">
@@ -24238,7 +24232,7 @@
         <v>83</v>
       </c>
       <c r="L161" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M161" s="13" t="s">
         <v>48</v>
@@ -24295,10 +24289,10 @@
     </row>
     <row r="162" spans="1:38" s="28" customFormat="1" ht="119.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="12" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B162" s="13" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C162" s="13"/>
       <c r="D162" s="14" t="s">
@@ -24321,10 +24315,10 @@
         <v>59</v>
       </c>
       <c r="K162" s="27" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="L162" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M162" s="13" t="s">
         <v>48</v>
@@ -24381,10 +24375,10 @@
     </row>
     <row r="163" spans="1:38" s="28" customFormat="1" ht="127.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B163" s="13" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C163" s="13"/>
       <c r="D163" s="14" t="s">
@@ -24410,7 +24404,7 @@
         <v>83</v>
       </c>
       <c r="L163" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M163" s="13" t="s">
         <v>48</v>
@@ -24467,10 +24461,10 @@
     </row>
     <row r="164" spans="1:38" s="28" customFormat="1" ht="107.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B164" s="13" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C164" s="13"/>
       <c r="D164" s="14" t="s">
@@ -24496,7 +24490,7 @@
         <v>83</v>
       </c>
       <c r="L164" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M164" s="13" t="s">
         <v>48</v>
@@ -24553,10 +24547,10 @@
     </row>
     <row r="165" spans="1:38" s="28" customFormat="1" ht="119.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B165" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C165" s="13"/>
       <c r="D165" s="14" t="s">
@@ -24582,7 +24576,7 @@
         <v>46</v>
       </c>
       <c r="L165" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M165" s="13" t="s">
         <v>48</v>
@@ -24639,10 +24633,10 @@
     </row>
     <row r="166" spans="1:38" s="28" customFormat="1" ht="122.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="12" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B166" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C166" s="13"/>
       <c r="D166" s="14" t="s">
@@ -24665,10 +24659,10 @@
         <v>159</v>
       </c>
       <c r="K166" s="27" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L166" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M166" s="13" t="s">
         <v>48</v>
@@ -24725,10 +24719,10 @@
     </row>
     <row r="167" spans="1:38" s="28" customFormat="1" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B167" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C167" s="13"/>
       <c r="D167" s="14" t="s">
@@ -24754,7 +24748,7 @@
         <v>83</v>
       </c>
       <c r="L167" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M167" s="13" t="s">
         <v>48</v>
@@ -24811,10 +24805,10 @@
     </row>
     <row r="168" spans="1:38" s="28" customFormat="1" ht="120.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="12" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B168" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C168" s="13"/>
       <c r="D168" s="14" t="s">
@@ -24837,10 +24831,10 @@
         <v>76</v>
       </c>
       <c r="K168" s="27" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="L168" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M168" s="13" t="s">
         <v>48</v>
@@ -24897,10 +24891,10 @@
     </row>
     <row r="169" spans="1:38" s="28" customFormat="1" ht="121.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B169" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C169" s="13"/>
       <c r="D169" s="14" t="s">
@@ -24926,7 +24920,7 @@
         <v>98</v>
       </c>
       <c r="L169" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M169" s="13" t="s">
         <v>48</v>
@@ -24983,10 +24977,10 @@
     </row>
     <row r="170" spans="1:38" s="28" customFormat="1" ht="111.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="12" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B170" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C170" s="13"/>
       <c r="D170" s="14" t="s">
@@ -25012,7 +25006,7 @@
         <v>60</v>
       </c>
       <c r="L170" s="20" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M170" s="13" t="s">
         <v>48</v>
@@ -25081,7 +25075,7 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:AL1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AL117" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>